<commit_message>
0.1.6: implement option for generateEmptyToJSON method.
</commit_message>
<xml_diff>
--- a/meta/listTarget/ApiTelegram.xlsx
+++ b/meta/listTarget/ApiTelegram.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectTs/meta/listTarget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4BEBC-1EAA-5D46-9FA9-03EC12495E19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00CA139-6E88-3748-A184-7BBAB2B18277}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12280" yWindow="5360" windowWidth="24320" windowHeight="14120" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,10 +41,19 @@
     <definedName name="必須" localSheetId="1">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="4"/>
@@ -54,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>クラス名</t>
   </si>
@@ -286,13 +295,45 @@
   <si>
     <t>blanco.restgenerator.telegrams</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>空のtoJSONメソッドを生成</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t xml:space="preserve">ジドウセイセイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>/* TypeScript 独自。 */</t>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">ドクジ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>telegramId</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>""</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>toJSONから除外</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -337,6 +378,11 @@
       <family val="2"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -376,7 +422,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -449,15 +495,6 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -851,7 +888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -867,51 +904,50 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -919,67 +955,67 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -987,19 +1023,23 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1412,10 +1452,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1426,36 +1466,44 @@
     <col min="6" max="6" width="6.83203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
     <col min="8" max="8" width="33.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19">
+    <row r="1" spans="1:12" ht="20">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="I1" s="80"/>
+    </row>
+    <row r="2" spans="1:12" ht="15">
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="I2" s="80"/>
+    </row>
+    <row r="3" spans="1:12" ht="15">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:12" ht="15">
+      <c r="I4" s="80"/>
+    </row>
+    <row r="5" spans="1:12" ht="15">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="I5" s="80"/>
+    </row>
+    <row r="6" spans="1:12" ht="15">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -1465,8 +1513,9 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="I6" s="80"/>
+    </row>
+    <row r="7" spans="1:12" ht="15">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1476,8 +1525,9 @@
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="I7" s="80"/>
+    </row>
+    <row r="8" spans="1:12" ht="15">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1487,31 +1537,34 @@
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:12" s="35" customFormat="1">
+      <c r="I8" s="80"/>
+    </row>
+    <row r="9" spans="1:12" s="34" customFormat="1" ht="15">
       <c r="A9" s="77" t="s">
         <v>39</v>
       </c>
       <c r="B9" s="78"/>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="75"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="35" t="s">
+      <c r="D9" s="74"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="34" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="35" customFormat="1">
-      <c r="A10" s="52" t="s">
+      <c r="I9" s="80"/>
+    </row>
+    <row r="10" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A10" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="76"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="B10" s="52"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="75"/>
+      <c r="I10" s="80"/>
+    </row>
+    <row r="11" spans="1:12" ht="15">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1523,8 +1576,9 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="I11" s="80"/>
+    </row>
+    <row r="12" spans="1:12" ht="15">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
@@ -1536,50 +1590,54 @@
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" s="35" customFormat="1">
-      <c r="A13" s="49" t="s">
+      <c r="I12" s="80"/>
+    </row>
+    <row r="13" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A13" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-    </row>
-    <row r="14" spans="1:12" s="35" customFormat="1">
-      <c r="A14" s="49" t="s">
+      <c r="I13" s="80"/>
+    </row>
+    <row r="14" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A14" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51" t="s">
+      <c r="B14" s="49"/>
+      <c r="C14" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-    </row>
-    <row r="15" spans="1:12" s="35" customFormat="1">
-      <c r="A15" s="49" t="s">
+      <c r="I14" s="80"/>
+    </row>
+    <row r="15" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A15" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51" t="s">
+      <c r="B15" s="49"/>
+      <c r="C15" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-    </row>
-    <row r="16" spans="1:12" s="35" customFormat="1">
-      <c r="A16" s="72" t="s">
+      <c r="I15" s="80"/>
+    </row>
+    <row r="16" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A16" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="73"/>
-      <c r="C16" s="51" t="s">
+      <c r="B16" s="72"/>
+      <c r="C16" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D16" t="s">
@@ -1588,362 +1646,414 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="I16"/>
+      <c r="I16" s="80"/>
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:10" s="35" customFormat="1">
-      <c r="A18" s="32" t="s">
+    <row r="17" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A17" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="72"/>
+      <c r="C17" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17" s="80"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+    </row>
+    <row r="18" spans="1:12" ht="15">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="I18" s="80"/>
+    </row>
+    <row r="19" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A19" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
-    </row>
-    <row r="19" spans="1:10" s="35" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="I19" s="80"/>
+    </row>
+    <row r="20" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A20" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-    </row>
-    <row r="20" spans="1:10" s="35" customFormat="1">
-      <c r="A20" s="52" t="s">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+      <c r="I20" s="80"/>
+    </row>
+    <row r="21" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A21" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="39"/>
-    </row>
-    <row r="21" spans="1:10" s="35" customFormat="1">
-      <c r="A21" s="52" t="s">
+      <c r="B21" s="52"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="38"/>
+      <c r="I21" s="80"/>
+    </row>
+    <row r="22" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A22" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="39"/>
-    </row>
-    <row r="22" spans="1:10" s="35" customFormat="1">
-      <c r="A22"/>
-      <c r="B22"/>
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:10" s="35" customFormat="1">
-      <c r="A23" s="32" t="s">
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="38"/>
+      <c r="I22" s="80"/>
+    </row>
+    <row r="23" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="I23" s="80"/>
+    </row>
+    <row r="24" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A24" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="56"/>
-    </row>
-    <row r="24" spans="1:10" s="35" customFormat="1">
-      <c r="A24" s="57" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="55"/>
+      <c r="I24" s="80"/>
+    </row>
+    <row r="25" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A25" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="58" t="s">
+      <c r="B25" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="59"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-    </row>
-    <row r="25" spans="1:10" s="35" customFormat="1">
-      <c r="A25" s="61"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="65"/>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" s="35" customFormat="1">
-      <c r="A26" s="61"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="65"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="58"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="59"/>
+    </row>
+    <row r="26" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A26" s="60"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
       <c r="H26"/>
-      <c r="I26"/>
+      <c r="I26" s="80"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10" s="35" customFormat="1">
-      <c r="A27" s="68"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="65"/>
+    <row r="27" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A27" s="60"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="64"/>
       <c r="H27"/>
-      <c r="I27"/>
+      <c r="I27" s="80"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10" s="35" customFormat="1">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-      <c r="F28"/>
-      <c r="G28"/>
+    <row r="28" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A28" s="67"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="64"/>
       <c r="H28"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="3" t="s">
+      <c r="I28" s="80"/>
+      <c r="J28"/>
+    </row>
+    <row r="29" spans="1:12" s="34" customFormat="1" ht="15">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29" s="80"/>
+    </row>
+    <row r="30" spans="1:12" ht="15">
+      <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A30" s="80" t="s">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="80"/>
+    </row>
+    <row r="31" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A31" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="80" t="s">
+      <c r="B31" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="79" t="s">
+      <c r="C31" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="79" t="s">
+      <c r="D31" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="79" t="s">
+      <c r="E31" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="79"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="80"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="79"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="15"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="19"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15" customHeight="1">
+      <c r="A32" s="79"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="76"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="76"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="29"/>
-      <c r="I32" s="15"/>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="15"/>
-    </row>
-    <row r="34" spans="1:9">
-      <c r="A34" s="19"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="15"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="15"/>
+      <c r="I32" s="81"/>
+    </row>
+    <row r="33" spans="1:9" ht="15">
+      <c r="A33" s="18">
+        <v>1</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="20"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="80" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="80"/>
+    </row>
+    <row r="35" spans="1:9" ht="15">
+      <c r="A35" s="18"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="80"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="15"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="22"/>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="19"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="15"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="22"/>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="19"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41" s="19"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="19"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="23"/>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="15"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="19"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="A46" s="24"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="15"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="22"/>
+    </row>
+    <row r="39" spans="1:9" ht="15">
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="80"/>
+    </row>
+    <row r="40" spans="1:9" ht="15">
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="80"/>
+    </row>
+    <row r="41" spans="1:9" ht="15">
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="22"/>
+      <c r="I41" s="80"/>
+    </row>
+    <row r="42" spans="1:9" ht="15">
+      <c r="A42" s="18"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="80"/>
+    </row>
+    <row r="43" spans="1:9" ht="15">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="80"/>
+    </row>
+    <row r="44" spans="1:9" ht="15">
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="80"/>
+    </row>
+    <row r="45" spans="1:9" ht="15">
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="80"/>
+    </row>
+    <row r="46" spans="1:9" ht="15">
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="22"/>
+      <c r="I46" s="80"/>
+    </row>
+    <row r="47" spans="1:9" ht="15">
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="27"/>
+      <c r="I47" s="80"/>
+    </row>
+    <row r="48" spans="1:9" ht="15">
+      <c r="I48" s="80"/>
+    </row>
+    <row r="49" spans="9:9" ht="15">
+      <c r="I49" s="80"/>
+    </row>
+    <row r="50" spans="9:9" ht="15">
+      <c r="I50" s="80"/>
+    </row>
+    <row r="51" spans="9:9" ht="15">
+      <c r="I51" s="80"/>
+    </row>
+    <row r="52" spans="9:9" ht="15">
+      <c r="I52" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="I31:I32"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E30:F31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D63" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1978,78 +2088,78 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="42" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="42" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="42" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="42" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="42" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="256" width="8.83203125" style="42" customWidth="1"/>
-    <col min="257" max="16384" width="10.83203125" style="42"/>
+    <col min="1" max="3" width="8.83203125" style="41" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="41" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="41" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="41" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="41" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="41" bestFit="1" customWidth="1"/>
+    <col min="11" max="256" width="8.83203125" style="41" customWidth="1"/>
+    <col min="257" max="16384" width="10.83203125" style="41"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="41" t="s">
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="41"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="42" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" s="44"/>
-      <c r="D4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="43"/>
+      <c r="D4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="J4" s="44"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="46" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="B6" s="48"/>
+      <c r="B6" s="47"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>

</xml_diff>